<commit_message>
post-tournament update for simulation of points
</commit_message>
<xml_diff>
--- a/euro_2021_poisson_forecast.xlsx
+++ b/euro_2021_poisson_forecast.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="54">
   <si>
     <t>Country</t>
   </si>
@@ -84,15 +84,15 @@
     <t>Sweden</t>
   </si>
   <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
     <t>Austria</t>
   </si>
   <si>
-    <t>Russia</t>
-  </si>
-  <si>
-    <t>Czech Republic</t>
-  </si>
-  <si>
     <t>Wales</t>
   </si>
   <si>
@@ -123,16 +123,19 @@
     <t>Team2_Goals</t>
   </si>
   <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
     <t>Group</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>L</t>
   </si>
   <si>
     <t>GF</t>
@@ -569,13 +572,13 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>0.1666666666666667</v>
+        <v>0.1724137931034483</v>
       </c>
       <c r="D2">
         <v>0.2</v>
       </c>
       <c r="E2">
-        <v>0.18118793511206</v>
+        <v>0.1823209705654847</v>
       </c>
       <c r="F2">
         <v>0.1818181818181818</v>
@@ -589,16 +592,16 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>0.1428571428571428</v>
+        <v>0.1282051282051282</v>
       </c>
       <c r="D3">
         <v>0.1666666666666667</v>
       </c>
       <c r="E3">
-        <v>0.1587849490662789</v>
+        <v>0.1526049288358287</v>
       </c>
       <c r="F3">
-        <v>0.1666666666666667</v>
+        <v>0.1538461538461539</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -615,7 +618,7 @@
         <v>0.1538461538461539</v>
       </c>
       <c r="E4">
-        <v>0.1378502237666865</v>
+        <v>0.1378626360117232</v>
       </c>
       <c r="F4">
         <v>0.1428571428571428</v>
@@ -629,13 +632,13 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>0.1086956521739131</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D5">
         <v>0.125</v>
       </c>
       <c r="E5">
-        <v>0.1134790383832921</v>
+        <v>0.1132606854575583</v>
       </c>
       <c r="F5">
         <v>0.1111111111111111</v>
@@ -649,13 +652,13 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>0.09803921568627452</v>
+        <v>0.1</v>
       </c>
       <c r="D6">
-        <v>0.125</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E6">
-        <v>0.1109704484387195</v>
+        <v>0.1089882787592535</v>
       </c>
       <c r="F6">
         <v>0.1111111111111111</v>
@@ -675,10 +678,10 @@
         <v>0.125</v>
       </c>
       <c r="E7">
-        <v>0.1078129459258913</v>
+        <v>0.10771286983693</v>
       </c>
       <c r="F7">
-        <v>0.1111111111111111</v>
+        <v>0.108187134502924</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -695,7 +698,7 @@
         <v>0.125</v>
       </c>
       <c r="E8">
-        <v>0.1111510279168876</v>
+        <v>0.1116134563179685</v>
       </c>
       <c r="F8">
         <v>0.1111111111111111</v>
@@ -709,13 +712,13 @@
         <v>12</v>
       </c>
       <c r="C9">
-        <v>0.05263157894736842</v>
+        <v>0.0510204081632653</v>
       </c>
       <c r="D9">
         <v>0.07692307692307693</v>
       </c>
       <c r="E9">
-        <v>0.06548336892623015</v>
+        <v>0.06432775814181695</v>
       </c>
       <c r="F9">
         <v>0.06666666666666667</v>
@@ -735,10 +738,10 @@
         <v>0.04347826086956522</v>
       </c>
       <c r="E10">
-        <v>0.0368754612447983</v>
+        <v>0.03735884582961044</v>
       </c>
       <c r="F10">
-        <v>0.03703703703703703</v>
+        <v>0.03846153846153846</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -752,10 +755,10 @@
         <v>0.02083333333333333</v>
       </c>
       <c r="D11">
-        <v>0.03448275862068965</v>
+        <v>0.08196721311475411</v>
       </c>
       <c r="E11">
-        <v>0.02724856688411723</v>
+        <v>0.03259758346069082</v>
       </c>
       <c r="F11">
         <v>0.02941176470588235</v>
@@ -769,13 +772,13 @@
         <v>15</v>
       </c>
       <c r="C12">
-        <v>0.01234567901234568</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="D12">
         <v>0.02941176470588235</v>
       </c>
       <c r="E12">
-        <v>0.01760514146782372</v>
+        <v>0.01801891772691372</v>
       </c>
       <c r="F12">
         <v>0.0196078431372549</v>
@@ -792,10 +795,10 @@
         <v>0.0131578947368421</v>
       </c>
       <c r="D13">
-        <v>0.0196078431372549</v>
+        <v>0.04761904761904762</v>
       </c>
       <c r="E13">
-        <v>0.01485125578644346</v>
+        <v>0.0182266671879753</v>
       </c>
       <c r="F13">
         <v>0.01492537313432836</v>
@@ -809,13 +812,13 @@
         <v>17</v>
       </c>
       <c r="C14">
-        <v>0.01052631578947368</v>
+        <v>0.01234567901234568</v>
       </c>
       <c r="D14">
-        <v>0.01492537313432836</v>
+        <v>0.0196078431372549</v>
       </c>
       <c r="E14">
-        <v>0.01259480792836844</v>
+        <v>0.01383794946938979</v>
       </c>
       <c r="F14">
         <v>0.01234567901234568</v>
@@ -829,16 +832,16 @@
         <v>18</v>
       </c>
       <c r="C15">
-        <v>0.0078125</v>
+        <v>0.009900990099009901</v>
       </c>
       <c r="D15">
         <v>0.0196078431372549</v>
       </c>
       <c r="E15">
-        <v>0.01170052952892936</v>
+        <v>0.01245353445718162</v>
       </c>
       <c r="F15">
-        <v>0.01098901098901099</v>
+        <v>0.01234567901234568</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -849,13 +852,13 @@
         <v>19</v>
       </c>
       <c r="C16">
-        <v>0.007692307692307693</v>
+        <v>0.008333333333333333</v>
       </c>
       <c r="D16">
         <v>0.01492537313432836</v>
       </c>
       <c r="E16">
-        <v>0.01089928391837362</v>
+        <v>0.01123156877363585</v>
       </c>
       <c r="F16">
         <v>0.01098901098901099</v>
@@ -869,16 +872,16 @@
         <v>20</v>
       </c>
       <c r="C17">
-        <v>0.005076142131979695</v>
+        <v>0.007936507936507936</v>
       </c>
       <c r="D17">
+        <v>0.02702702702702703</v>
+      </c>
+      <c r="E17">
+        <v>0.01289866931792124</v>
+      </c>
+      <c r="F17">
         <v>0.01234567901234568</v>
-      </c>
-      <c r="E17">
-        <v>0.009309232937107058</v>
-      </c>
-      <c r="F17">
-        <v>0.009900990099009901</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -889,16 +892,16 @@
         <v>21</v>
       </c>
       <c r="C18">
-        <v>0.00625</v>
+        <v>0.006329113924050633</v>
       </c>
       <c r="D18">
-        <v>0.01492537313432836</v>
+        <v>0.02325581395348837</v>
       </c>
       <c r="E18">
-        <v>0.01070323548530411</v>
+        <v>0.009075313776216476</v>
       </c>
       <c r="F18">
-        <v>0.009900990099009901</v>
+        <v>0.007936507936507936</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -909,16 +912,16 @@
         <v>22</v>
       </c>
       <c r="C19">
-        <v>0.005263157894736842</v>
+        <v>0.005882352941176471</v>
       </c>
       <c r="D19">
+        <v>0.01234567901234568</v>
+      </c>
+      <c r="E19">
+        <v>0.009439604103564056</v>
+      </c>
+      <c r="F19">
         <v>0.009900990099009901</v>
-      </c>
-      <c r="E19">
-        <v>0.007230469493979656</v>
-      </c>
-      <c r="F19">
-        <v>0.007936507936507936</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -935,7 +938,7 @@
         <v>0.007936507936507936</v>
       </c>
       <c r="E20">
-        <v>0.006242799012464616</v>
+        <v>0.006588187952245041</v>
       </c>
       <c r="F20">
         <v>0.006622516556291391</v>
@@ -949,13 +952,13 @@
         <v>24</v>
       </c>
       <c r="C21">
-        <v>0.00398406374501992</v>
+        <v>0.002493765586034913</v>
       </c>
       <c r="D21">
-        <v>0.006622516556291391</v>
+        <v>0.01204819277108434</v>
       </c>
       <c r="E21">
-        <v>0.004711631163323779</v>
+        <v>0.005186033208946653</v>
       </c>
       <c r="F21">
         <v>0.004975124378109453</v>
@@ -969,13 +972,13 @@
         <v>25</v>
       </c>
       <c r="C22">
-        <v>0.001331557922769641</v>
+        <v>0.001237623762376238</v>
       </c>
       <c r="D22">
         <v>0.006622516556291391</v>
       </c>
       <c r="E22">
-        <v>0.002485643012088236</v>
+        <v>0.002473658104011439</v>
       </c>
       <c r="F22">
         <v>0.001996007984031936</v>
@@ -995,7 +998,7 @@
         <v>0.00398406374501992</v>
       </c>
       <c r="E23">
-        <v>0.002487670019435637</v>
+        <v>0.002371348812196974</v>
       </c>
       <c r="F23">
         <v>0.002493765586034913</v>
@@ -1009,13 +1012,13 @@
         <v>27</v>
       </c>
       <c r="C24">
-        <v>0.001331557922769641</v>
+        <v>0.001996007984031936</v>
       </c>
       <c r="D24">
-        <v>0.003322259136212625</v>
+        <v>0.00398406374501992</v>
       </c>
       <c r="E24">
-        <v>0.002049218129992337</v>
+        <v>0.002124771264793244</v>
       </c>
       <c r="F24">
         <v>0.001996007984031936</v>
@@ -1029,16 +1032,16 @@
         <v>28</v>
       </c>
       <c r="C25">
-        <v>0.001298701298701299</v>
+        <v>0.00131578947368421</v>
       </c>
       <c r="D25">
         <v>0.004975124378109453</v>
       </c>
       <c r="E25">
-        <v>0.003194136048156153</v>
+        <v>0.003030416325545076</v>
       </c>
       <c r="F25">
-        <v>0.003067484662576687</v>
+        <v>0.002493765586034913</v>
       </c>
     </row>
   </sheetData>
@@ -1048,13 +1051,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
@@ -1067,8 +1070,11 @@
       <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1079,13 +1085,16 @@
         <v>16</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1096,13 +1105,16 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1113,13 +1125,16 @@
         <v>23</v>
       </c>
       <c r="D4">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1130,13 +1145,16 @@
         <v>15</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1152,8 +1170,11 @@
       <c r="E6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1164,13 +1185,16 @@
         <v>23</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1181,13 +1205,16 @@
         <v>13</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1198,13 +1225,16 @@
         <v>25</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1212,16 +1242,19 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1232,13 +1265,16 @@
         <v>25</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1246,16 +1282,19 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1263,21 +1302,24 @@
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -1286,44 +1328,53 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1334,13 +1385,16 @@
         <v>27</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1351,13 +1405,16 @@
         <v>18</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1373,8 +1430,11 @@
       <c r="E19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1382,16 +1442,19 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1405,10 +1468,13 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1419,47 +1485,56 @@
         <v>24</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>3</v>
+      </c>
+      <c r="F23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
         <v>24</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1470,13 +1545,16 @@
         <v>24</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1490,10 +1568,13 @@
         <v>4</v>
       </c>
       <c r="E26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1504,13 +1585,16 @@
         <v>11</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1524,10 +1608,13 @@
         <v>2</v>
       </c>
       <c r="E28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1538,13 +1625,16 @@
         <v>11</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1555,13 +1645,16 @@
         <v>19</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1572,13 +1665,16 @@
         <v>19</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1589,13 +1685,16 @@
         <v>9</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1606,13 +1705,16 @@
         <v>26</v>
       </c>
       <c r="D33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1623,13 +1725,16 @@
         <v>10</v>
       </c>
       <c r="D34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1645,8 +1750,11 @@
       <c r="E35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1657,13 +1765,16 @@
         <v>10</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1677,7 +1788,10 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1698,7 +1812,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>34</v>
@@ -1710,16 +1824,16 @@
         <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1727,28 +1841,28 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>8</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
         <v>7</v>
-      </c>
-      <c r="I2">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1756,28 +1870,28 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <v>4</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1785,28 +1899,28 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H4">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1814,28 +1928,28 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G5">
         <v>9</v>
       </c>
       <c r="H5">
-        <v>-6</v>
+        <v>-4</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1843,28 +1957,28 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>-1</v>
+        <v>15</v>
       </c>
       <c r="I6">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1872,28 +1986,28 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
         <v>6</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
       <c r="H7">
-        <v>6</v>
+        <v>-4</v>
       </c>
       <c r="I7">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1901,86 +2015,86 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H8">
-        <v>-6</v>
+        <v>-9</v>
       </c>
       <c r="I8">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <v>3</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="I9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G10">
         <v>9</v>
       </c>
       <c r="H10">
-        <v>-8</v>
+        <v>3</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1988,7 +2102,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -2000,13 +2114,13 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="I11">
         <v>9</v>
@@ -2017,28 +2131,28 @@
         <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F12">
         <v>2</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="I12">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -2046,28 +2160,28 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G13">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <v>-6</v>
       </c>
       <c r="I13">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -2078,54 +2192,54 @@
         <v>35</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G14">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H14">
         <v>-4</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15">
         <v>6</v>
       </c>
-      <c r="G15">
-        <v>7</v>
-      </c>
       <c r="H15">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="I15">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2136,25 +2250,25 @@
         <v>35</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I16">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -2168,22 +2282,22 @@
         <v>1</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G17">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H17">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -2191,28 +2305,28 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G18">
         <v>2</v>
       </c>
       <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18">
         <v>6</v>
-      </c>
-      <c r="I18">
-        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -2220,28 +2334,28 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H19">
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="I19">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -2249,28 +2363,28 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H20">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="I20">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -2278,28 +2392,28 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G21">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H21">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="I21">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -2307,28 +2421,28 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H22">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I22">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -2336,7 +2450,7 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -2348,13 +2462,13 @@
         <v>1</v>
       </c>
       <c r="F23">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I23">
         <v>6</v>
@@ -2365,7 +2479,7 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -2380,10 +2494,10 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H24">
-        <v>-12</v>
+        <v>-8</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -2394,28 +2508,28 @@
         <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F25">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H25">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="I25">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2436,7 +2550,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>34</v>
@@ -2448,31 +2562,31 @@
         <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -2480,28 +2594,28 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>8</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
         <v>7</v>
-      </c>
-      <c r="I2">
-        <v>6</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -2512,42 +2626,33 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G3">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H3">
-        <v>-6</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
         <v>2</v>
       </c>
       <c r="N3">
@@ -2556,43 +2661,34 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="I4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J4">
-        <v>2</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>-1</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N4">
         <v>3</v>
@@ -2600,31 +2696,31 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H5">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -2635,10 +2731,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -2650,13 +2746,13 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I6">
         <v>9</v>
@@ -2670,43 +2766,34 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <v>3</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J7">
         <v>2</v>
-      </c>
-      <c r="K7">
-        <v>3</v>
-      </c>
-      <c r="L7">
-        <v>2</v>
-      </c>
-      <c r="M7">
-        <v>4</v>
       </c>
       <c r="N7">
         <v>2</v>
@@ -2714,10 +2801,10 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2729,28 +2816,19 @@
         <v>2</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H8">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="I8">
         <v>3</v>
       </c>
       <c r="J8">
-        <v>2</v>
-      </c>
-      <c r="K8">
-        <v>3</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N8">
         <v>3</v>
@@ -2761,40 +2839,31 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H9">
-        <v>-6</v>
+        <v>-9</v>
       </c>
       <c r="I9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J9">
-        <v>2</v>
-      </c>
-      <c r="K9">
-        <v>3</v>
-      </c>
-      <c r="L9">
-        <v>-2</v>
-      </c>
-      <c r="M9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N9">
         <v>4</v>
@@ -2805,7 +2874,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -2817,13 +2886,13 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="I10">
         <v>9</v>
@@ -2837,10 +2906,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -2852,13 +2921,13 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G11">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I11">
         <v>6</v>
@@ -2872,10 +2941,10 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2887,13 +2956,13 @@
         <v>2</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="I12">
         <v>3</v>
@@ -2907,10 +2976,10 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -2922,10 +2991,10 @@
         <v>3</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H13">
         <v>-8</v>
@@ -2948,25 +3017,25 @@
         <v>35</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I14">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -2977,31 +3046,31 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G15">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H15">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J15">
         <v>2</v>
@@ -3012,7 +3081,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>35</v>
@@ -3027,10 +3096,10 @@
         <v>2</v>
       </c>
       <c r="F16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G16">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H16">
         <v>-4</v>
@@ -3041,40 +3110,58 @@
       <c r="J16">
         <v>3</v>
       </c>
+      <c r="K16">
+        <v>3</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
       <c r="N16">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
         <v>35</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G17">
         <v>6</v>
       </c>
       <c r="H17">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J17">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>-1</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
       </c>
       <c r="N17">
         <v>4</v>
@@ -3082,16 +3169,16 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -3100,13 +3187,13 @@
         <v>8</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I18">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -3117,31 +3204,31 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
         <v>6</v>
-      </c>
-      <c r="H19">
-        <v>-3</v>
-      </c>
-      <c r="I19">
-        <v>4</v>
       </c>
       <c r="J19">
         <v>2</v>
@@ -3152,10 +3239,10 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -3170,10 +3257,10 @@
         <v>2</v>
       </c>
       <c r="G20">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H20">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="I20">
         <v>3</v>
@@ -3187,31 +3274,31 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G21">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H21">
-        <v>-2</v>
+        <v>-8</v>
       </c>
       <c r="I21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J21">
         <v>4</v>
@@ -3225,40 +3312,31 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H22">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I22">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J22">
         <v>1</v>
-      </c>
-      <c r="K22">
-        <v>3</v>
-      </c>
-      <c r="L22">
-        <v>1</v>
-      </c>
-      <c r="M22">
-        <v>3</v>
       </c>
       <c r="N22">
         <v>1</v>
@@ -3269,7 +3347,7 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -3281,28 +3359,19 @@
         <v>1</v>
       </c>
       <c r="F23">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I23">
         <v>6</v>
       </c>
       <c r="J23">
-        <v>1</v>
-      </c>
-      <c r="K23">
-        <v>3</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N23">
         <v>2</v>
@@ -3313,40 +3382,31 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F24">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H24">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="I24">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J24">
-        <v>1</v>
-      </c>
-      <c r="K24">
-        <v>3</v>
-      </c>
-      <c r="L24">
-        <v>-1</v>
-      </c>
-      <c r="M24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N24">
         <v>3</v>
@@ -3357,7 +3417,7 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -3372,10 +3432,10 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H25">
-        <v>-12</v>
+        <v>-8</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -3405,7 +3465,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>34</v>
@@ -3417,89 +3477,80 @@
         <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="I2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J2">
-        <v>2</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>-1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N2">
         <v>3</v>
       </c>
       <c r="O2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3511,28 +3562,19 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H3">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="I3">
         <v>3</v>
       </c>
       <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N3">
         <v>3</v>
@@ -3543,10 +3585,10 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3558,13 +3600,13 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="I4">
         <v>3</v>
@@ -3576,12 +3618,12 @@
         <v>3</v>
       </c>
       <c r="O4">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>35</v>
@@ -3596,10 +3638,10 @@
         <v>2</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H5">
         <v>-4</v>
@@ -3610,19 +3652,28 @@
       <c r="J5">
         <v>3</v>
       </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
       <c r="N5">
         <v>3</v>
       </c>
       <c r="O5">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -3637,10 +3688,10 @@
         <v>2</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H6">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="I6">
         <v>3</v>
@@ -3652,7 +3703,7 @@
         <v>3</v>
       </c>
       <c r="O6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -3660,40 +3711,31 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="I7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>3</v>
-      </c>
-      <c r="L7">
-        <v>-1</v>
-      </c>
-      <c r="M7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N7">
         <v>3</v>
@@ -3729,7 +3771,7 @@
         <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3737,19 +3779,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3760,13 +3802,13 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -3780,13 +3822,13 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -3797,16 +3839,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -3817,16 +3859,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -3843,10 +3885,10 @@
         <v>9</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -3866,10 +3908,10 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3877,19 +3919,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3919,7 +3961,7 @@
         <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3927,19 +3969,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3950,10 +3992,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -3967,19 +4009,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3987,16 +4029,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -4029,7 +4071,7 @@
         <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -4037,7 +4079,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -4057,19 +4099,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -4099,7 +4141,7 @@
         <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -4110,10 +4152,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>

</xml_diff>